<commit_message>
Merge met error in 'delete'
</commit_message>
<xml_diff>
--- a/res/vragen-uit-excel.xlsx
+++ b/res/vragen-uit-excel.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="21600"/>
   </bookViews>
   <sheets>
-    <sheet name="hierKomtMaincategory" r:id="rId3" sheetId="1"/>
+    <sheet name="hierKomtMaincategory" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t>MeerkeuzeVraag</t>
   </si>
@@ -93,17 +100,59 @@
   </si>
   <si>
     <t>Converteert één interface naar een andere</t>
+  </si>
+  <si>
+    <t>Is Tamo leuk?</t>
+  </si>
+  <si>
+    <t>Is Georges cool?</t>
+  </si>
+  <si>
+    <t>Is Ruben grappig?</t>
+  </si>
+  <si>
+    <t>Is Sam supercool?</t>
+  </si>
+  <si>
+    <t>Welke omschrijving past het best bij Sam?</t>
+  </si>
+  <si>
+    <t>Tof</t>
+  </si>
+  <si>
+    <t>Ongelofelijk cool, interessant, grappig, gespierd, ….</t>
+  </si>
+  <si>
+    <t>Cool</t>
+  </si>
+  <si>
+    <t>Grappig</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,7 +163,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -126,26 +175,368 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="7">
+    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Normaal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="4" width="16.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2"/>
-    <row r="3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -168,18 +559,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7">
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="n">
-        <v>1.0</v>
+      <c r="C4">
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -202,18 +593,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7">
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="n">
-        <v>1.0</v>
+      <c r="C6">
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -224,18 +615,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7">
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="n">
-        <v>1.0</v>
+      <c r="C8">
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -246,29 +637,29 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7">
       <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" t="n">
-        <v>2.0</v>
+      <c r="C10">
+        <v>2</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7">
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" t="n">
-        <v>2.0</v>
+      <c r="C11">
+        <v>2</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -291,18 +682,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:7">
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" t="n">
-        <v>1.0</v>
+      <c r="C13">
+        <v>1</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -322,18 +713,146 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:7">
       <c r="B15" t="s">
         <v>19</v>
       </c>
-      <c r="C15" t="n">
-        <v>2.0</v>
+      <c r="C15">
+        <v>2</v>
       </c>
       <c r="D15" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>